<commit_message>
Get daily reddit data: Tue May 13 08:12:51 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_18.xlsx
+++ b/data/collected_data/2025_05_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C487"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3168 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1klg2zq</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Scared of removing Press on Nails – Any Advice?</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1klg2zq/scared_of_removing_press_on_nails_any_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1klf8j9</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>How to avoid skin peeling around nails and make them stronger</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klf8j9</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1klf6jl</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Snek</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klf6jl</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1kl5na3</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Broken Nail Matrix?</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kl5na3/broken_nail_matrix/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1kldr0t</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Mermaid Nails</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ay1bceueh0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1kldqaa</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>oh look, a strawberry!</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kldqaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1kldo12</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>I did gel x nails as</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kldo12/i_did_gel_x_nails_as/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1klcp06</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Started doing my nails at home. This is my second set, what can I improve?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klcp06</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1klde0i</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>TW/ when a little too crazy trimming my cuticles</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/suqhtwazah0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1klcxk6</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>spring nails!</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95ruc5h26h0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1klbwb5</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Birthday Set - Cow Print 🐄🤠</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klbwb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1kl7lbh</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Can (soft?) gel polish prevent your nails from bending backwards?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kl7lbh/can_soft_gel_polish_prevent_your_nails_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1kl6lit</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Can anyone tell me what causes this? It looks like some sort of stress mark.</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wk9e5n06lf0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1klb0av</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>New nails and new shape!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klb0av</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1kl9uwh</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Buggy nails!</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl9uwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1kl96ff</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>i can’t tell if i like the nude and need help figuring out what to do</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mbwy2sw17g0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1kla0ov</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Work in 3D🌸🫧🤍</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kla0ov</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1kl920l</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>DIY gel X 🩷💛</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl920l</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1kl8no2</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl8no2</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1kl8llh</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>My boyfriend pays for my nails to be done before we go on a trip, not knowing that... 😳</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl8llh</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1kl868i</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>🚨 Buyer Beware: My Experience with Sistaco 🚨</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kl868i/buyer_beware_my_experience_with_sistaco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1kl8fbj</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>My new set. What do we think?</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl8fbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1kl88ac</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Dremel on a regular manicure?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kl88ac/dremel_on_a_regular_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1kl7y9c</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Really loving this look</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nozavmfdwf0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1kl7uhr</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>first time doing successful cat eye :3</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mivhiyehvf0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1kl7tz5</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Bright and cheery</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl7tz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1kl7ju9</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Which shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ck0ygi91tf0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1kl7hii</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Perfect Blue 💙</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nzi41qnhsf0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1kl59ai</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>As a nail-biter, I'm always anxious to get my nails done. This time, I don't regret it at all.</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl59ai</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1kl7btj</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>I am SO ready for my cruise this week now.</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl7btj</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1kl6vf1</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Long lasting press ons?</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kl6vf1/long_lasting_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1kl6h9d</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>can’t go wrong with french tips</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/weud1kh7kf0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1kl6dso</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Did my nails yesterday 😌</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xak6jmmfjf0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1kl69ab</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>April showers bring May flowers..</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/igqapb7fif0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1kl624l</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Is it weird to close your eyes during a pedicure?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kl624l/is_it_weird_to_close_your_eyes_during_a_pedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1kl60pu</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>First time using blooming gel and I really like the results!</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xxrzatigf0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1kl50yd</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Wedding Press-Ons</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvyz65iu8f0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1kl4r28</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Stuck some gems on I found in the arts and crafts section of the supermarket 🛒🌺🌸🏪</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v187ciot6f0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1kl4q4a</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>I love green</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl4q4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1kl4dww</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>First time in a salon</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qw20uvi74f0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1kl49uf</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Amo estas uñitas</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iurst1wd3f0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1kl43zw</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>First time trying something other than a solid color, what do you think?</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl43zw</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1kl43qv</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>First time trying something other than a solid color, what do you think?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl43qv</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1kl42md</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>For peeps who get gel</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kl42md/for_peeps_who_get_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1kl3nqa</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Could it be the blooming gel</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xskujvd2ze0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1kl3fgz</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Did this set myself, wdyt?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl3fgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1kl3et2</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>2 months Growth of my Nails</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl3et2</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1kl2osy</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Miffy nails</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bke14i6se0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1kl2ki1</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Spring Vibes</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl2ki1</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1kl2i9b</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Does almond suit my hands? Want to make sure before I get them redone tomorrow! 🩷</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl2i9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1kl2a3o</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Magic Remover for Gel/Builder Removal</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kl2a3o/magic_remover_for_gelbuilder_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1kl260i</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Which looks better</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl260i</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1kl1yq5</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>My most recent set! Love the look of two different hands</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl1yq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1kl0qyv</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Matte?</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl0qyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1kkxsbp</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Possible allergy?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kkxsbp/possible_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1kky8f1</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Builder Gel, Hard gel VS soft gel?</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1e5lxvd8xd0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1kkylly</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>can i use press ons</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkylly</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1kkzpix</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>beginner but proud</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jbprqbad7e0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1kkzsb0</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Is it weird to still ask for regular mani/pedis at nail salons?</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kkzsb0/is_it_weird_to_still_ask_for_regular_manipedis_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1kl1it5</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>I wanted to be "fashionable" so I got my nails done and it ruined my natural nails 😔</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9d26950ke0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1kkzm9k</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Pink, pearly &amp; soft. I'm really in love with them.</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkzm9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1kl1c3q</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Angel's feathers</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl1c3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1kl1bad</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Top coat not shiny after one day?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kl1bad/top_coat_not_shiny_after_one_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1kl0rsj</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Fresh Mint</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwxe964tee0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1kl0ojy</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Nail beds December 24 thru May 25</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl0ojy</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1kkyhqu</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Reposting, as it was taken down as not my work. It is my work. I just used an Instagram pic from Instagram, @cmknails_ I also shared my admin page from Instagram that shows it's mine.</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkyhqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1kkyyxn</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>My new love 😍</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8gle6pa2e0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1kkya81</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Asking for advice</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkya81</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1kkxzeh</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Lily Pads with a touch of Disney  ! Can you spot the Mickey Mouse head ? 👀</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkxzeh</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1kkxyik</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>I'm so obsessed with these! 💅</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehu5kkr9vd0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1kkx52w</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Gel vs Acrylic?</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9p4dp8lpd0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1kkwtst</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>What is the half circle at the front of my nail?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08ky6zx3nd0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1kkwfjg</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Composition on My second set of nails?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkwfjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1kkis5p</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>How do you keep getting gel nails extensions?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kkis5p/how_do_you_keep_getting_gel_nails_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1kkkny0</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Can someone please tell me if this color is possible with gel polish? Credit to KXAMELIE on Amazon</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/424i67rica0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1kklabu</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>[Show &amp; Tell] Dreamy Princess Chrome Nails — With Polygel + Builder Gel Overlay for Strength + Heavy 3D Embellishments</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DJio5phPCL8/?igsh=MWJyNmJvZmZmZmUxbA==</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1kkvnuu</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Help what do i do to fix it?</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kkvnuu/help_what_do_i_do_to_fix_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1kkwc3z</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Meow 😸 how do you rate my new work?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkwc3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1kkkzck</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Is there a way to keep my nails after I take them off?</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74xifw3aga0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1kkezxy</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>How to regrow after Onycholysis ?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kkezxy/how_to_regrow_after_onycholysis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1kkn314</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>does anyone know a colour similar to this?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkn314</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1kkw68s</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>I made my own nail oil pen today!</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eg7hextxid0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1kkvh8i</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>gel nail newbie</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkvh8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1kkv7qx</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>My favourite shade and I am obsessed with this .</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkv7qx</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1kkv73u</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>nailed it with this glam combo! ౨ৎ˚⟡˖ ࣪</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkv73u</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1kkv4sl</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Nail tip too wide?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kkv4sl/nail_tip_too_wide/</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1kkuvnt</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>So obsessed with these 😍</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2sgptvm9d0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1kkupub</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Can I make Gel X type extensions work for my uneven nails?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hd6wb4jh8d0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1kkumsm</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Help finding product</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjjtkqot7d0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1kkujev</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Is this a good nail drill?</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brx2gdi77d0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1kkucp4</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Challenged myself to try and make 100% biodegradable press-ons! Using Re:soil nail tips made from cellulose based resin; Pine resin for nail adhesive; and Common greenshield lichen.</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkucp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1kkuciv</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>I always cut my nails very short, but recently I grew them and today tried filing them. How did I do with shaping them? Any advice/feedback/changes before I try nail polish?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkuciv</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1kku624</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Zodiac nails!!!</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kku624</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1kktpd0</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>To add more white or to not add more white</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kktpd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1kktitz</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>I need help 😭</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kktitz</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1kktbcq</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>my progress on myself (5 months)</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kktbcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1kkr8ri</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>spring nails 💅</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4kat8i5hc0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1kkphki</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Swirl!</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkphki</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1kkp8v6</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Screenshot it</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9xqag8m4xb0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1kkom98</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Pink floral nails</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dx2in4zzpb0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1klf967</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Best Cuticle Products + Super Dry Fingertips/Top of Nail Help</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1klf967/best_cuticle_products_super_dry_fingertipstop_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1klezfl</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Rediscovering my new (old) favourite hobby and wanted to share</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0fltyyssh0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1kleonh</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>a pink jelly more pigmented than cirque rosewater?</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kleonh</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1kldsaz</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Trying to capture all the colours of Hush. (Having a hard time uploading videos for some reason, final attempt...)</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gre98uk8fh0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1klclvl</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>If it ain’t a holographic magnetic, I don’t want it!</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hh0bveou2h0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1klc7o3</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>lunar eclipse - cadillacquer</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klc7o3</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1klbvrl</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>An attempt at teal glass nails</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klbvrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1klbvcv</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>r/RedditLacqueristas Mentioned 🗣️</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dw2egfvnvg0f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1klbtm4</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Did you all hear Pete Buttigieg on Smartless Podcast today?</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://podcasts.apple.com/us/podcast/smartless/id1521578868?i=1000705999165</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1kl9okm</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>I’m so in love with this stunner!</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kg1rgskjbg0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1kl9k7d</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Let’s get shifty!🩷💚</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5z4rs2liag0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1kl9aft</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Replacement fan brushes for Seche Vite/Vive?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kl9aft/replacement_fan_brushes_for_seche_vitevive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1kl9756</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Ink bleed / marble nails 💙</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kl9756/ink_bleed_marble_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1kl8wdv</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>My Storage Solution!</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mj6a2chk4g0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1kl8vhe</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Anyone know of a good orange to white/cream thermal?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kl8vhe/anyone_know_of_a_good_orange_to_whitecream_thermal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1kl7kzu</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Magnetic Polish Issue</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kl7kzu/magnetic_polish_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1kl7fgq</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Magnet position?</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djvftx90sf0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1kl6t1b</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>For those wondering why international stockists aren’t restocking Mooncat</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ks8entumf0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1kl6sdf</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>I Had Never Found The Right Shade Of Red Until Today</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl6sdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1kl6p7p</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>colour recommendations for this shade of blue?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl6p7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1kl6ib9</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>looking for this dnd colour</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykwgmmlgkf0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1kl6ds0</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Bkl I will be your undoing</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kl6ds0/bkl_i_will_be_your_undoing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1kl4ws9</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>So I went with ILNP</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2h531rz7f0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1kl3cmm</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Mooncat Hardcore Base &amp; Nail Damage</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kl3cmm/mooncat_hardcore_base_nail_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1kl34z0</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Flowers that matched my sunset-themed skittle 🥰</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0uelab8cve0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1kl3174</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Fire 🔥 &amp; Ice 🧊</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3538fjylue0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1kl2mdd</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Fairycore is just as amazing as I expected it to be🩵🧚🏻☁️</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl2mdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1kl2j9b</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>ILNP Price Increase Effective May 29</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kl2j9b/ilnp_price_increase_effective_may_29/</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1kl2gmd</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>The Shiftiness of BKL Choose Life</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yljovsdkqe0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1kl1xd7</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Glitter grabber recs? Preferably available on Amazon bc I have credit there rn.</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kl1xd7/glitter_grabber_recs_preferably_available_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1kl1ky1</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>My turn for tragedy</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57qwcckfke0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1kl1kl4</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Dissimulation🌈💜</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r7wh0r0ake0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1kl17q4</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Mother's Day grandma inspired nails</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl17q4</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1kl14hz</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Skittles 🤪🌈</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uvraot8he0f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1kl11vt</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>My First Sassy Sauce Foray (with a wee bit of Mooncat's Foxfire)</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl11vt</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1kl0y5s</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Life-long cuticle picker that has never taken care of or painted my nails - where do I start?!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l31seyszfe0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1kl0v9t</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Shifty shorties!</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl0v9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1kl0pa6</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>can (and should I) do gel x / hard gel on chipped toe nail?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kl0pa6/can_and_should_i_do_gel_x_hard_gel_on_chipped_toe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1kl0fze</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>I usually don’t wear bright colors but lately I’ve really been enjoying it!</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2k96x3ghce0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1kl0974</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Tried to dupe BKL the chosen one is chosen for evil</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ji7lt9q5be0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1kkzz1k</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Talk me out of buying these</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bubblyc89e0f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1kkzxvn</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>You Do Lou</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkzxvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1kkzpi2</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Looking for warmer / peachier version of MC Fake Halo</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkzpi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1kkzh78</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Sinners inspired mani</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkzh78</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1kkzccf</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Peachy gold goodness</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kshkrmhp4e0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1kkz850</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Sometimes the lighting is just too perfect</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dngos3o14e0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1kkyk7p</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Tried to dupe BKL the chosen one is chosen for evil</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r9w86tdczd0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1kkxp7c</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Lumen - Glass Frog 🐸</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yr4netgltd0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1kkwqow</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Mermaid Bait</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkwqow</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1kkvtjb</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>My husband agreed to let me paint his nails for the first time - I did mine to match!</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkvtjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1kkvhvo</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Magnetic polish and Magnets help!</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kkvhvo/magnetic_polish_and_magnets_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1kkv3nm</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Was going to have plain purple but I'm glad I added the stars</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zgu65gh9bd0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1kkuv3h</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Pretty in Pearls</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xudz7vzi9d0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1kkuuja</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>I’m sorry I ever doubted Essie Gel-Setter</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ys8lf9ue9d0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1kkulm0</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>How long does it take for y’all’s nails to dry completely?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y96pdm3n7d0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1kkukp6</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Nonbinary Galactic!</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52xbxtyg7d0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1kkukd4</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Pocket cuticle oil pen</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kkukd4/pocket_cuticle_oil_pen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1kktzv0</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Your nails but better frenchies</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kktzv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1kkt6z5</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Accidental vibe match</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wumuva7bxc0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1kkt4j1</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Lost in the darkness, you will be found</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkt4j1</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1kkt42l</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>House of Hades Troubleshooting</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/toy1rupnwc0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1kkrc18</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Mother's day mani + new swatch book 😍</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkrc18</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1kkkewc</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>What polish did I actually get? La Colors</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkkewc</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1kkme4w</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Why is my nail line (idk what its called) so receded? How do i fix it?</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09o28mk6xa0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1kkqoi8</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Springy Shimmery Mani for May</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkqoi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1kkqk5h</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Ilnp Aspen - would you wear it in springtime?</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkqk5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1kkppv9</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Blow your socks off Blue - Kathleen &amp; Co. “It’s Showtime!”</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkppv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1kkoq6w</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kkoq6w/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1kknzay</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Set inspired by my beloved everyday bag</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kknzay</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1klfb7o</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Been messing with nail foil glue and these nail foils does anyone have any advice</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlms41qnwh0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1kldhis</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Another set for myself</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6hrvo80ch0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1klbods</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Fruity Summer Nails</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9uht4jxttg0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1kla6fn</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>New Set I did.</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kla6fn</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1kla5d1</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>French tips on tips!</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kla5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1kla3t6</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>need help figuring out my jellycat dragon nail set</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kla3t6</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1kl9jhi</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>sakura flowy glowy pearly on top of magnetic gel</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0r10lzbag0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1kl8nvn</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>All set for EDC!</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9krkmtag2g0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1kl623q</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>First time making flowers, how’d I do?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl623q</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1kl2th0</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>help me decide</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl2th0</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1kl19f2</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Purple chrome, middle finger reminds me of a dinosaur</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl19f2</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1kl18d4</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Angel's feathers</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl18d4</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1kl0pzc</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Purple Frenchie's with fruit</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kl0pzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1kl0eub</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Fishing Lure Nails 😍</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbykapx9ce0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1kkzxpa</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>DIY Hydrangeas</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kkzxpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1kkpso2</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Spring florals</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jmw14253c0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1kknq27</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Set inspired by my beloved everyday bag</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kknq27</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed May 14 08:12:40 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_18.xlsx
+++ b/data/collected_data/2025_05_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C487"/>
+  <dimension ref="A1:C676"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8712,6 +8712,3219 @@
         </is>
       </c>
     </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1km8l0z</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Nail art on my puppy cause she doesn’t mind 🩷 I did the watermelon French tips the rest were done by her groomer  (all pet safe)</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km8l0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1km7ohg</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Some without polish and long, what do you think?</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zt49ezkcqo0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1km7io8</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Marbling Style</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a168utagoo0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1km7468</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>did my bf’s nails</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km7468</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1km5qrm</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>What’s wrong with my nails?</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km5qrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1km5jwc</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>What’s a simple appropriate  gift for my manicurist?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1km5jwc/whats_a_simple_appropriate_gift_for_my_manicurist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1km58q3</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Inspo from fxncy_nxails on Pinterest 🔥✨</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lf1xpqek0o0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1km5gbz</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Tortoiseshell attempt 🐢</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4qqderm2o0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1km5bra</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>My Finger Nail Rings</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7q5p6qd1o0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1km59s4</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Tried doing a gel manicure w/ tips at home—need advice!</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1km59s4/tried_doing_a_gel_manicure_w_tips_at_homeneed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1km4th4</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>whats the trick to making cuticles look good</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6sw3hwewn0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1km4s9t</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1km4s9t/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1km4is0</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Newbie</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6whsjjutn0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1km446w</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>My nail btoke for the first time and im devastated</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km446w</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1km3pbw</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Love how my natural nails turned out 💅</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4gm86y9mn0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1km3ifg</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Fresh set inspired by forest fungi 🌲 🍄 🌳</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5k3dvhjkn0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1km3fcy</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>ask for acrylic, gel x, or dip powder? (ref photo from CcstrStudio on Etsy)</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dj7xqmqrjn0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1km3d88</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Are my nailbeds flat or curved? I can't tell</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km3d88</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1km374a</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Lemons for the summer 💛🍋</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km374a</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1km2k6r</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Advice on cleaning nailed while new nail grows?</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km2k6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1km2ca6</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Molten Metal 🩶</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vzxbkonp9n0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1km293u</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Cutesy Press-On Nails</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/saxu0yg59n0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1km1ywv</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>finally looking after my natural nails instead of getting fake ones! looking gorgeous 💕</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8it719nk6n0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1km1ye7</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Can I use gel liners over top of regular nail polish?</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1km1ye7/can_i_use_gel_liners_over_top_of_regular_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1km1stq</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Spring to summer set</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km1stq</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1km0jyf</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>First time GelX Nails. Is it supposed to look like that? Did I damage my index finger?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n1hyvjaium0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1klufxg</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>PSA to all the Baddies with gel nails</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1klufxg/psa_to_all_the_baddies_with_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1kltcum</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>is this normal? SNS manicure showing cracks / less than a week</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kltcum</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1km1okx</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>I've always been a squoval girl, but I'm loving almond now that my nails are getting longer!</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpcgymo14n0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1kloqab</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Guys help me decide if this is pink or purple</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kloqab</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1klzmh1</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>We do recover!! 😆💕</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bcn4dywmm0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1km1n5y</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>i need tips and constructive criticism!</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km1n5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1klopr1</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>press on recs?</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpkbis58hk0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1klrlsn</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>proposal nails!</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klrlsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1klsf9v</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Situation with my nails trying to open a tricky door</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1klsf9v/situation_with_my_nails_trying_to_open_a_tricky/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1klxw3u</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>UV aging damage?!</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1klxw3u/uv_aging_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1km16yr</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Mango nails 🥭</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1fh5ve5wzm0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1klnuw4</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Pastel Ultraviolet</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klnuw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1km1i5b</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Gel product without filing?</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1km1i5b/gel_product_without_filing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1km121p</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>The first time my nail tech took a pic of my nails afterwards 😅 rate them 🌸</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9vqiqiqym0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1km11jy</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Nail shape?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7nuzfamym0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1km0wri</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>sweet siren of the cove vibes 🫧🧜🏽‍♀️</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km0wri</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1km0q8h</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>She back after 6.5 weeks! 😳</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km0q8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1km0nkt</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Obsessed with these kiss press ons</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km0nkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1km0e9z</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Tampa gel-x nail tech plug</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km0e9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1klzh9x</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Qué color es más combinable para uñas ?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1klzh9x/qué_color_es_más_combinable_para_uñas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1klzf8m</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>love it!</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3cvt0c8clm0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1klzdl7</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Is there any shape I can shape my short nails into other than a natural shape?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m51axtezkm0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1klyrb9</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Update to my previous post- the nail color!</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klyrb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1klxysu</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>White Gel Polish... makes me want to cry.</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1klxysu/white_gel_polish_makes_me_want_to_cry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1klxw8b</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>What is the thinnest overlay that will keep my nail strong?</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fztre9is9m0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1klxlbo</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>SpongeBob nails! 🧽🦀🐿️</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klxlbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1klwrul</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Out of my comfort zone</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klwrul</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1klwrei</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Just starting with an at home gel kit! 1st attempt vs 2nd attempt!</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klwrei</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1klwfvv</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Beee you tee full</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klwfvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1klvkeh</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>nail drill help!!</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1klvkeh/nail_drill_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1klvd25</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Proper Way to Remove Dip Mani</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pozidp2vrl0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1kluqf0</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>nail day is my favourite day</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbcsg8v9nl0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1klt3l7</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Decided to do a dark red french tip at my appointment today and I’m kind of in love</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0inx5c1xbl0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1klstx2</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Pink on moss + bonus lichen</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klstx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1klsqxl</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Black dip with gel designs</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klsqxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1klsdk7</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>May Nails🍓🍋</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/my6whrcw6l0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1kls4u1</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Oh, don't mind me. Just showin' off a few flattering night pics of my shiny white French tips. 📸😉😁😍✨️💕🤍</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kls4u1</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1klrlbm</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>1 week going on almost 2 weeks of no chipping/breaking. Other than growth, polish is still on 😀</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klrlbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1klrki3</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>guy here. just finished getting my toes done. Danny boy blue+ gloss topcoat 💙</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7jh57ra1l0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1klr9ai</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Just had my first set of acrylics removed</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klr9ai</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1klr8hs</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>I liked the color and with sparkles</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5xfgrpyyk0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1klr7xi</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>I feel bad, but…</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1klr7xi/i_feel_bad_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1klqtjv</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>A Happy set 😊</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klqtjv</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1klqr75</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Builder gel: what am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1klqr75/builder_gel_what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1klqj7l</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Pokémon Type Nails</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abuye4v2uk0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1klq8g5</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Beginner here! My Gel nails will easily peel off if I pick at them, why?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1klq8g5/beginner_here_my_gel_nails_will_easily_peel_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1klq565</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>🕷️🐛Bugs🐛🪲</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klq565</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1klpvfi</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Absolutely Love My Neon Nails</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klpvfi</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1klpqum</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Builder Gel Fills</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1klpqum/builder_gel_fills/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1klpitv</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Acrylic Newbie</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klpitv</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1klpbp2</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Out of comfort zone nails I did to myself 🩶</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klpbp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1klp7p1</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>What am I doing Wrong?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klp7p1</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1klp57y</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Nails from Mexico City!</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wivkil8akk0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1klot88</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>I always gravitate toward green.</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4norkaxhk0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1klonq9</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Mother’s Day nails, not my usual look because they are for my mom ❤️</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgczyx7tgk0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1klo94o</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Love a vibrant red</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klo94o</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1klo50h</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>ugh love my nails</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ry0u759dk0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1klns05</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1klns05/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1kleotb</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Help Idk if i should cancel</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ari0qqncph0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1klmqj5</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Shoutout to the girlie who went to Thailand for the nail inspo ✨</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljdv1fg23k0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1klnaud</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>This took 3 hours, should I not have done hard gel?</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klnaud</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1klnp8v</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>First ever attempt at gels</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/marl4ol0ak0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1kllanv</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Press Ons I made</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kllanv</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1kln8pc</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>🌺</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vjb44rp6k0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1klmbfk</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Arlecchino claws. My tech went feral 🖤❤️</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3fy8su2uzj0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1klm6k8</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Celestial silver cat eye😍 im in love</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klm6k8</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1kllyp9</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Need Advice- Nail Art molds too narrow?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kllyp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1kllprs</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Gel colour popped off - best quick fix?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9883abn1vj0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1kllnmm</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Bug Nails</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9c0z3skuj0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1kll1zc</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>neutral opaque gel polish?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kll1zc/neutral_opaque_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1klk52o</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>are dog nails allowed?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klk52o</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1klk1g2</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Does anyone here suffer from OCD involving their nails/hands?</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umregebogj0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1klju1x</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>1,2,3,4,5 witch one is yr favorite 💅🙀😻</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klju1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1kljefi</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>✨✨✨</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpvjew6daj0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1km9p8z</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Down the gel rabbit hole</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1km9p8z/down_the_gel_rabbit_hole/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1km8ns8</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Stress-swatched some random untrieds while watching The Last Of Us</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y9thc0542p0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1km8d0i</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>How to make this polish less streaky</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km8d0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1km8ak3</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Polishes like frequent flyer</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1km8ak3/polishes_like_frequent_flyer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1km7u51</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Is there any reason I shouldn't use acetone from the hardware store as nail polish remover?</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1km7u51/is_there_any_reason_i_shouldnt_use_acetone_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1km7prd</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>DVN yucca in bloom and cirque Luna</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/np7jplqrqo0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1km716s</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Maybe some of you friends remember my princess, Cher, from my post a while back with her fancy nails! Her groomer outdid herself this time and I wanted to share 🩷 (WATER-BASED PET SAFE)</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km716s</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1km6h55</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Bees Knees Lacquer</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km6h55</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1km5v1k</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>First attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km5v1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1km5hmw</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>What is happening to my tips 😭</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iisy2svy2o0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1km5gk7</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Found this glitter EXPLOSION for $2.50, plus a collection of glowy blue comparisons</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km5gk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1km58ku</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>The last time I heard you laugh</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4leuupi0o0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1km4of3</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Dupe of Cirque Ridge Filler color?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km4of3</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1km4lv6</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>What's your favorite matte topcoat?</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1km4lv6/whats_your_favorite_matte_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1km4aou</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>We do recover 😂💕</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vhwwaorrn0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1km49j5</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Florals? For Spring? Groundbreaking.</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km49j5</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1km3yqy</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>whole lotta lurid lately</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km3h2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1km3wpy</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>DND is currently having a sale for $4.50 a bottle 🗣️🗣️🗣️</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1km3wpy/dnd_is_currently_having_a_sale_for_450_a_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1km3w0z</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>My friend called them "witchy"</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km3w0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1km3gq0</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>⭐️ please I’m a staaaarrrrrrrr ⭐️</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km3gq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1km2y91</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>I just love this sparkly pink</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bt829mrffn0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1km2pam</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for Sassy sauce’s Pop.Yew.Lar</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9su3ph6dn0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1km23g4</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Advertising</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1km23g4/advertising/</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1km220h</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Summery jelly gradient! 🍉</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szopaw8c7n0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1km1o6k</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Ocean Water 💦 Rogue Lacquer</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km1o6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1km1kew</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Milk &amp; Lilac 🥛🪻</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pjy08k513n0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1km1jk9</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Okay yeah, BKL does make incredible magnetics</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fdikra2u2n0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1km0niy</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Latest update on the LBOH/AI/Sugar Bubbles issue</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8q5wcw9dvm0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1km0fzt</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>KBshimmer reflective glitters</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km0fzt</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1km0c0w</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>The most cheerful and genuinely sweet polish!</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km0c0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1km09n1</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>How to Apply Nail Polish for Someone With Tremors?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1km09n1/how_to_apply_nail_polish_for_someone_with_tremors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1kly3tr</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Nail art is intimidating for lots of reasons, but I wasn’t going to let my shorties be one of them! Inspired by Monet’s paintings of water lilies.</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kly3tr</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1klx5kb</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Mixed Berries 🍒🍓🫐(2.0)</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klx5kb</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1klwv9j</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Something different for me</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klwv9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1klwtkk</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>cuticula moonlit is a good dupe for holo taco cowboy tears</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klwtkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1klwd9k</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Absolutely loving the flakies!!!</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ij1a6p1yyl0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1klvqof</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Go-To Polishes for the Indecisive?</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1klvqof/goto_polishes_for_the_indecisive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1klveu0</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Does anyone know how often Polished For Days have sales?</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1klveu0/does_anyone_know_how_often_polished_for_days_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1klv0sm</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Color combination brought to you by my nasty bruise 🩵</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0drs2qtdpl0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1klugtg</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - Out On Your Street 🪴🪴</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klugtg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1klu7ua</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>The rainbows are calling you 🌈</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klu7ua</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1klu2zj</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Neon might be dulling a bit?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0889ac0nil0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1klt9hj</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Blacklight Neons</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1klt9hj/blacklight_neons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1klt5ur</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Grad nails! 🤘🧡</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klt5ur</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1klt2or</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Meeting Distraction</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zf5ntloqbl0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1klt03a</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Red Eyed Lacquer: Coming For Your Coins</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9u6j2v58bl0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1klsv44</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Essie Clambake - 2025 rerelease. It’s TOO orange</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aiamngh7al0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1klslu0</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>I looove ILNP Flower Child</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klslu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1klsk69</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Mother Duck said “Quack Quack Quack!” And four little ducks came waddling back! 🦆🦆🦆🦆</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klsk69</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1klsfzy</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>My DIY version of the DVN Dust to Dust collection</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klsfzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1kls2g2</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Best QDTC</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ferylbbt4l0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1klryqk</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Magnetic | Flakie Split Mani</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tmwtqku24l0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1klrgis</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>in love with pandemonium by mooncat</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klrgis</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1klrdqb</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>What would go good with this dress?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jns226xyzk0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1klqo5y</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>After The Rain ☔️</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klqo5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1klimno</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Perfect Pink-Purple Quest</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b84fe5aq1j0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1klq9zu</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Relaxing greens</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1klq9zu/relaxing_greens/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1klpfy1</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Polishes like this?</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klpfy1</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1kloyr3</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Norpsilocin slays</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kloyr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1klos77</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>What I wore in April</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klos77</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1kloguf</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>We love a color shift!</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kloguf</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1klodgv</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>layering base coats question</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1klodgv/layering_base_coats_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1klo9ph</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>My First Ever Halos - Obsessed!</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1pk5ci4ek0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1klo0p4</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Pastel Ultraviolet ✨️</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klo0p4</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1klmmbk</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>A classic for a reason 💜</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klmmbk</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1klkbjc</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Flakies Sandwich</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klkbjc</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1klk1n6</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Serum of Seduction</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klk1n6</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1kljqog</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>I couldn’t even wait after cleaning up the edges!</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5qjtenxjoi0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1kljake</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Drown My Demons swatch</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctdrtkl89j0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1kli5e5</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Spreadsheet advice sought</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kli5e5/spreadsheet_advice_sought/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1kl53p9</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Help me find the perfect green pls</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mw3il7f9f0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1km7x4w</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Sculpting Bone Nails is fun</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjyauiu6to0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1km6d35</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>I have a problem</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iroyloyqbo0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1km65tu</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Today I was inspired by my marble tablecloth and used blooming gel with primary colors</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km65tu</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1km4ayr</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Celestial set by @nailsbysaraii_ on insta</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xouu4g7urn0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1km3gmd</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>I’m trying to learn how to do gradients. Any tips for a newbie?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ti4bquf2kn0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1km31s5</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>✨🍓Berries for this month's set</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/teacwikbgn0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1km2gvx</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Molten Metal 🩶</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5uu5tvlvan0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1km2fcv</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Buzz buzz</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km2fcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1km0omh</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Ribcage nail!</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovzfmh7mvm0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1km0e8v</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Made a fun little Coraline set for myself yesterday!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2btmow7tm0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1klzewf</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Sailor Moon customs ✨</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klzewf</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1klx209</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Help me decide if this is pink or purple</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1klx209</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1klufu3</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Spring is in the air 💟🪻</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90e727i5ll0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1klu6qa</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Trying new things to practice, how'd i do? Advice?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kg6k6y0fjl0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1klscoq</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>May Nails🍓🍋</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/go5fgasq6l0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1klp8im</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Blinged Up</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kf2glfezkk0f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1klo2uo</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>third set i ever made!</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tmyzlgtck0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1kkmvz5</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Cherry cola</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qlolxuvj3b0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu May 15 08:12:54 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_18.xlsx
+++ b/data/collected_data/2025_05_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C676"/>
+  <dimension ref="A1:C857"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11925,6 +11925,3083 @@
         </is>
       </c>
     </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1kn2qv7</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>I’m a beginner nail tech and this is my first gel polish manicure!</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcw9q07ckw0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1kn2is5</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Mix n' match design! 🙈</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn2is5</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1kn0okz</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Help! Is pearl chrome supposed to look like this?</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/676rk5o0vv0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1kmzkf0</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Keryflex oh</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmzkf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1kmzdsg</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Less is more for this girl</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmzdsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1kmzayg</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>spring manicure</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9o36u5t1gv0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1kmz9l5</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Just wanted to brag on my nail tech!!</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmz9l5</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1kmykfj</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Help with cuticle care</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmykfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1kmyu7i</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Baby Take a Vow🎀🫧</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hoxlmzggbv0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1kmysoe</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Just popped off my acrylics</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykjj1q61bv0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1kmymq4</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>How to make my salon gel manicure last longer? Extra clear top coats at home?</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kmymq4/how_to_make_my_salon_gel_manicure_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1kmym95</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>This flower matches my nails 🧡🩷</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ief82b999v0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1kmud44</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>I need desperate help with my nails/cuticles</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1iae6406u0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1kmto59</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Builder gel at home?</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kmto59/builder_gel_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1kmqw5g</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>How to explain shape to tech?</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmqw5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1kmvjvi</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Where do I find blank press-on nails or gelx nails this short? (Photo is from chi.nail_ on Instagram)</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e93it4dqgu0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1kmv074</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Is this dip nail kit the same as regular gel?</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ru95txsmbu0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1kmy5ru</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Short Nail Beds Hellllp ~inspo by Çiŷdem on Pinterest</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmy5ru</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1kmxjpu</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Matte purple with accent nail</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjqxy6z0zu0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1kmus97</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>What shape? Or keep them?</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44wqqp6o9u0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1kmx7dr</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>a couple of sets that i’ve done in the last month. 😊  don’t mind the dry hands!</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmx7dr</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1kmwwe2</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Lil french</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmwwe2</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1kmwqc3</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Nails for a Friend</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmwqc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1kmwpwi</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>My little sister is learning to do acrylic nails</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmwpwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1kmwotb</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Obsessed with the tomato</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmwotb</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1kmw809</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>??????? what</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmw809</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1kmvofh</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Trying out a new color!</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/osbstwouhu0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1kmvkcm</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Everytime</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmvkcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1kmv59o</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Natural Nail Colours?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmv59o</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1kmv13h</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>No he podido encontrar el nombre de este diseño 😭</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0nez06yubu0f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1kmv0e8</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Just wanted to share my new nails</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmv0e8</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1kmuq6p</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>First time wearing nail polish as a man</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9q62b2c69u0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1kmup30</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>I hate the way my left hand came out! CCW</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmup30</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1kmudor</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>bubble bath chrome 🫧</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmudor</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1kmubbr</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>How do we feel about square nails?</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xue88agk5u0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1kmu3tc</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>design vs completion :3</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmu3tc</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1kmttw5</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Italian pink from DND 🎀</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmttw5</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1kmtogp</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>My nail tech always delivers</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmtogp</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1kmtkq2</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Pink glitter micro French 🩷</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmtkq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1kmrg44</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>The first set of gel press ons I’ve made. Inspired by my favourite hockey team. They aren’t perfect, but I’m proud of them</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1naj073it0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1kmt1t3</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>New set, matching pedi ❤️</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxhq1ylvut0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1kmszw5</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Semi permanent arctic fox stained on my beauty white French tips</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmszw5</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1kmsu4l</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Is there a way to combine regular nail polish with a gel polish base and/or top coat to make it last longer? 🤔</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kmsu4l/is_there_a_way_to_combine_regular_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1kmsit9</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>can i use acrylic to put on gel x or press ons?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kmsit9/can_i_use_acrylic_to_put_on_gel_x_or_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1kmri3j</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Pastel French 💅</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b64abxbiit0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1kmr2cj</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Silver Ocean Nails</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmr2cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1kmqktq</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Going natural. Just a normal gel manicure this time!</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cj50s0wobt0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1kmq22c</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>new 💢💢 nails</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sh3yabmw7t0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1kmpv1g</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Almond French.</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cd825ghh6t0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1kmptfy</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Is It Still Safe To Get a Manicure?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kmptfy/is_it_still_safe_to_get_a_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1kmpo19</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>classy red nails 💅💅💅</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6n6m94w25t0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1kmphfn</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Summer Flower set. Anyone like flower nails ?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmphfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1kmpak8</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Cherry season 🍒</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtbw8knd2t0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1kmfxme</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>At home nails! (Not qualified)</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pulvg9to7r0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1kmlozs</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Discoloration - help</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmlozs</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1kmozjj</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Which one looks better? Ombre or no?</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmozjj</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1kmojn1</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Sun’s out ☀️</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfbyx9cyws0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1kmohwc</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Builder gel/polygel/gel polish</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kmohwc/builder_gelpolygelgel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1kmo5cy</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Absolutely Stunning Nail Art by @cutenailstudio in Austin</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38xvbj84us0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1kmo2w6</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>First time trying dual form poly gel nails – beginner advice?</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kmo2w6/first_time_trying_dual_form_poly_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1kmny6v</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Chrome Sherbet 🍧</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5mgd49cjss0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1kmnt9w</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>I need your opinions. (Please read description)</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmnt9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1kmnk3t</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Natural tone</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6e2qgnvtps0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1kmn9aw</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Bright shorties!</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmn9aw</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1kmn1n3</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>I will never get tired of cat eye polish.</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmn1n3</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1kmmjft</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Oil soaking seems to be working, but my nails still seem damaged?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmmjft</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1kmmja8</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Just a guy who’s obsessed with builder gel manicures.</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmmja8</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1kmm4pe</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Nail changed color in one spot?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmm4pe</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1kmm1cn</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>What looks better on me, round/almond or squoval?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmm1cn</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1kmltdw</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Are these too thick? It’s done with hard gel</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmltdw</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1kmlssd</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Little love potion nails 💅</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmlssd</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1kml8jf</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Terminology question</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kml8jf/terminology_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1kml292</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>more clear pictures of my prom nails :)))</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kml292</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1kmky9r</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>my sets always seem to be thick at the cuticle and then thick at the tip. what am i doing wrong?</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmky9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1kmkxfy</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Vampire vibes</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmkxfy</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1kmktzb</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>I just love a lot of charms😭🥹</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmktzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1km6iva</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Nails dirty??</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1km6iva</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1kmkipt</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>ISO affordable full-cover gel tips!</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kmkipt/iso_affordable_fullcover_gel_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1kmjsu7</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>underside edges of my natural nail separating from biab :(</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmjsu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1kmjvrr</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Destined for Short Nails</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykkpjzi00s0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1kmjonz</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Obsessed with my new nail design — too extra or just enough?</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgsb7ienyr0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1kma582</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>I want to try a new nail gel the Jin.B thick gel. Does anyone know if it lasts on short and more thin nails?</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kma582/i_want_to_try_a_new_nail_gel_the_jinb_thick_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1kmbohk</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Potential eczema around my eyelids, worried that my acrylics are triggering it…are there any alternatives to acrylics?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kmbohk/potential_eczema_around_my_eyelids_worried_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1kmj6p5</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>my prom nails:)))</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c72e16i3vr0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1kmj5kn</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>my very first set i’ve painted!</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qadzs7vur0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1kmff56</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>acrylic overlay vs builder gel/structured hard gel</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kmff56/acrylic_overlay_vs_builder_gelstructured_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1kmi0ng</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>I put a gel top coat on my dip at home and now my nails are tacky and smudged</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ek2guqxrmr0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1kmj424</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>My latest press on set :’)</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4dy3ulkur0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1kmdqqm</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Nails burn like they’ve been dipped in lava when put in the lamp</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kmdqqm/nails_burn_like_theyve_been_dipped_in_lava_when/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1kmir2d</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>🏳️‍⚧️ Showing off my new Sprummer  Nails 🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmir2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1kmijze</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Can I pull off taupe?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmijze</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1kmij46</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>☁️ dreamy ☁️</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmij46</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1kmhxeo</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>✨️Fabulous✨️</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmhxeo</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1kmhqvd</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>What would be the best nail type to get?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kmhqvd/what_would_be_the_best_nail_type_to_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1kmgxnw</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>I was feeling something floral</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orqkui61fr0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1kmfzqz</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Press ons are the best</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmfzqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1kmfygo</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>I just really like how these turned out 😁🦋</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lll2vzlu7r0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1kme1mp</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Any recommendations for nail polishes (non-gel and gel) for beginners?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kme1mp/any_recommendations_for_nail_polishes_nongel_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1kmdc3q</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>LPS press ons :)</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmdc3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1kmd5cv</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Obsessed with my French ombré!</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmd5cv</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1kn2g5d</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>I wish someone would make an IG nail account of various indie polish manicures specifically under *hospital lighting*. There are so many health care workers and people who otherwise spend time in hospitals who wonder what various polishes will look like under the bright hospital lighting!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kn2g5d/i_wish_someone_would_make_an_ig_nail_account_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1kn252n</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>any way to make these look thinner?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn252n</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1kmz43e</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>I matched my dinner to my nails 💅</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmz43e</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1kmyw1t</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Phoenix Queen</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqvsxmizbv0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1kmyv24</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Aussie accessible Dupes for mooncat fake halo &amp; I’m a MF Supernova</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kmyv24/aussie_accessible_dupes_for_mooncat_fake_halo_im/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1kmysv6</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Ilnp Sabrina</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqasvvr2bv0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1kmyrkd</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Essie fans, I need some guidance please</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kmyrkd/essie_fans_i_need_some_guidance_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1kmxoe1</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>What’s everyone using as tools instead of their nails?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kmxoe1/whats_everyone_using_as_tools_instead_of_their/</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1kmwv16</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Mani improvements</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kmwv16/mani_improvements/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1kmwr3i</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Had to order from Dimension Nails at least one more time before they close this month 😔</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmwr3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1kmvo79</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Am I Everything You Fear</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmvo79</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1kmviii</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Love Reading</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmviii</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1kmvdkk</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Help! Looking for a gel top coat that won’t stain.</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/coypnv03fu0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1kmuz95</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>cracked polish jewel of the ball</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wncg2fldbu0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1kmutxi</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>OPI wicked collection really slapped</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmutxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1kmuqs5</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>wearing red to vent my rage 🩸</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmuqs5</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1kmum3d</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>When the top coat smears your nail art 🥲</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmum3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1kmug7p</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Nail Care is Self Care 😊</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmug7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1kmtdy8</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Nichibotsu reminds me of Clionadh's Norpsilocin</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmtdy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1kmt7qv</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for this colour!</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kmt7qv/looking_for_a_dupe_for_this_colour/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1kmt50k</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Cracked - Home by 9 from April PPU</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rgwusb8kvt0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1kmt4nf</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Mooncat's Millennia! I think I'm finally figuring out how to get a decent cat eye.</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mue99i6qut0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1kmt4j5</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>My first "real" manicure and first polish in years.</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kmt4j5/my_first_real_manicure_and_first_polish_in_years/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1kmsz93</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Hand Cream Recommendations</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4d8lta5but0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1kmrhgc</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>My nail grows kind of weird, I don’t know how to fix it</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmrhgc</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1kmrbcv</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>shining like a new penny</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmrbcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1kmqqjh</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Am I developing nail blindness</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmqqjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1kmqksn</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Non-gel dupe?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zc5o47npbt0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1kmqded</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Searching for new Indie brands</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kmqded/searching_for_new_indie_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1kmprum</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Updates! (We aren’t raising our prices)</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmprum</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1kmp6f8</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>does anyone have any ideas as to how i can fix this nail?</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ewosz4k1t0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1kmnotc</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Fake Halo</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqwljs8sqs0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1kmnjpo</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Maelstrom really is THAT polish</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmnjpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1kmlc4j</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Flower Dance 🌸</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmlc4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1kmkcei</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Showing off my new Sprummer Rock Candy Nails</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmkcei</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1kmkaec</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Mooncat Ultrahot</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmkaec</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1kmjpf9</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Types of shimmers?</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmjpf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1kmjnck</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>some competition for the sunny spot today.</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmjnck</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1kmjaoo</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Periwinkle with a Twinkle ✨️✨️✨️</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/qaggkOu</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1kmj2t2</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>ILNP-Isabella 💙💙</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovh79wpbur0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1kmj1i6</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>I can't look away</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chqipwe2ur0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1kmit48</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Mooncat price increase</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s556sodhsr0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1kmimsp</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Glass Rose</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/042tp2o8rr0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1kmia5n</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Mooncat pricing update!</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlm6am2qor0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1kmhy8q</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Indigo Bananas!</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmhy8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1kmhwi0</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Glow in the dark holo anyone? 🤍</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmhwi0</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1kmh9l0</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Enchanted by enchantment</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmh9l0</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1kmglp2</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Taming the Fox</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmglp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1kmgc8k</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Floral season 🌸🏵🌺</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmgc8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1kmgbf8</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Corporate bathroom lighting</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8rh53jbar0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1kmfyxq</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Starry Eyed Treachery 💎</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmfyxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1kmftqf</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>The Sorrow of Your Empty Seat</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmftqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1kmf3az</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>ILNP Jet Setter</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmf3az</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1kmayxk</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Nail beds have shrunk after Biab removal?</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmayxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1kn1pw7</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Swirly whirly</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rbi9az7i7w0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1kmzhiw</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Did Pokémon Nailz</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rbyugg02iv0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1kmyo64</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Got a cute set of stiletto nails :)</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmyo64</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1kmxi9c</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>New Technique I'm working on</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmxi9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1kmxdoj</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>What do you guys think of my Furina nails</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmxdoj</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1kmw819</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Ocean</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7868tc7wmu0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1kmvva1</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Attempt 2 at gutty works nails!</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87kada3mju0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1kmvfeq</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>🧿</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3z80dpkkfu0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1kmuzzh</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>What do you think of this ombre technique?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mtq2j6ukbu0f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1kmso91</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Why does my cat eye gel turn yellow when magnetized?</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kmso91/why_does_my_cat_eye_gel_turn_yellow_when/</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1kmsklc</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>A happy set 😊 by Kristin @ luxx nails</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmsklc</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1kmr7me</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>What do you think of the designs for boys, would you make them?</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0po1tkbgt0f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1kmr559</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>A few attempts at rose nails- matte or glossy top? Help is welcome</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmr559</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1kmr0tx</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Silver Ocean Theme</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmr0tx</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1kmpiuf</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>More practice.</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0r3ccnd14t0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1kmpc7r</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Maybe I’ll have better luck on this sub. (More in description)</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmpc7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1kmo2uy</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>My first nail art “beam me up”</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmo2uy</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1kmnwty</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Chrome Sherbet 🍧</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rhax87n7ss0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1kmnhyr</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Blessed Lady nails ❤️</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmnhyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1kmmxhp</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>The latest set i made inspired by impressionism</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmmxhp</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1kmm7el</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>These were so fun 🌸</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28il2w39gs0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1kmgng3</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Getting to paint some super fun sets this week 😍💅💛</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmgng3</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1kmea69</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Summers almost here🙌🏻😀 artist is the goat of Philly @sueznails</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmea69</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1kmdepx</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>LPS press ons :)</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmdepx</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1kmdczn</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Joan Miro nails</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z51lwxkamq0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1kmbyno</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Super fun custom set for a festival!</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xaqg9m9z7q0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1kmaedd</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>hangyodon and hello kitty nails i did</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kmaedd</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri May 16 08:12:33 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_18.xlsx
+++ b/data/collected_data/2025_05_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C857"/>
+  <dimension ref="A1:C1042"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15002,6 +15002,3151 @@
         </is>
       </c>
     </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1knuwje</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>First design on myself!</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2cabla5ci31f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1knu2j9</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Very natural looking color combo</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5z07pfj5831f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1kntbbb</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>a sip of love..</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/065uj1i2z21f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1knspyv</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Really happy with how clean my characters are coming out! Here is Goro Sajuro ☺️</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xow1gocs21f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1knrtl5</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Beginner here! Need some advices and tips.</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1knrtl5/beginner_here_need_some_advices_and_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1knrdwb</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Are there any problems?</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/raqmlotpe21f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1knrchr</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Tips on healthy nails.</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knrchr</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1knqxet</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>classic red 💅</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knqxet</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1knqsve</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Quick reshape/update to my nails that grow crazy fast</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knqsve</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1knoebc</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Shape?</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knoebc</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1knoie3</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>High Honor vs Low honor 🦌🐺</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knoie3</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1knqp9p</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Mushroom French tip! 🍄❤️🍃</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knqp9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1knppmt</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Do my nails grow fast?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/niutg6fiy11f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1knpzld</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Do these look bad? First time getting builder gel</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knpzld</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1knpjq0</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Fresh set (on myself)</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knpjq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1knphc4</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knphc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1knph5q</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knph5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1knp7j7</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Progress pictures with my sets</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knp7j7</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1knozz6</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Do nail soaking bowls really work?</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1knozz6/do_nail_soaking_bowls_really_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1kniser</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Has anyone else been having problems with OPIs new Gel formula??!</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kniser/has_anyone_else_been_having_problems_with_opis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1knlb3a</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Nail grows out weirdly</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knlb3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1knntcc</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Bubbling and peeling of shellac?</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knntcc</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1kno5rf</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Sexc red nails 😋❤️</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z76og8j3k11f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1kno361</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Beautiful nails I loved them🍒🏁</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mjx8jgcej11f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1knnoci</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Slowly getting the hang of it</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knnoci</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1knnd64</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>First time doing my own acrylics.</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eiy2qunoc11f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1knnak3</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Obsessed!!!</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knnak3</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1knna0b</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Vacay Ready</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knna0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1knn10q</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>This blue 🥹</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knn10q</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1knmyil</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>I’ve been too embarrassed to go back to the salon</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knmyil</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1knmy78</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>I’ve been too embarrassed to go back to the salon</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knmy78</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1knmqma</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Did a blue set after a long time. Let me know if you guys wanna see me wearing them</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knmqma</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1knkfsw</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Normal growth? When do get redone for vacation..</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knkfsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1knl7uf</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>IT BROKE!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knl7uf</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1knmo3v</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Finally used Molten Sky</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knmo3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1knkv68</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>1 day after mani</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ov187gdr01f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1knj03f</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Tried something new (to me)</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knj03f</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1knkddo</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Did cat eye for the first time and kind of hate them</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knkddo</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1knk718</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>How does this apex look? Too high?</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knk718</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1knjgp9</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Love this set</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9w5fy30rg01f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1kniz0s</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>What about tattooed nails? My new work 🍒🦋</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2kn9tu7d01f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1kngfmv</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Am I being unreasonable?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kngfmv</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1kn3j96</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>My fourth time doing my nails</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13mqtzjluw0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1knhcu9</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Third attempt at doing my own nails, Holiday inspired!</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knhcu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1knigl9</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>why are nail salons often so careless about your time :(</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1knigl9/why_are_nail_salons_often_so_careless_about_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1knicmr</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Good brand recommendations for gel polish? The one I’m using now is very streaky and hard to work with</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1knicmr/good_brand_recommendations_for_gel_polish_the_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1knhqvx</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>NEW NEW</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b25yhcz8401f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1knhkfv</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>after months of being careful...</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/stzxz2ov201f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1knhirl</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Custom nail decals? I'm trying to commission custom dice, which the decals are stuck to.</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1knhirl/custom_nail_decals_im_trying_to_commission_custom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1knhimd</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>New nails. Classic red.</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wdvkg0k201f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1knhf35</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Is this MMA?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cs4ugrqr101f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1knh9ap</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>I did my girls nails for her graduation :)</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74e6nkmm001f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1kngv47</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Baroque almost killed me</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kngv47</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1knguzb</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>What shape fits me best?</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/077txmsnxz0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1kngefv</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>New celestial set 🌙 💫 ✨</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oih5jj8cuz0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1kng8kj</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>I broke my nail at work!!</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4exy6nr5tz0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1kng38y</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>third set by me</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kng38y</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1knfyg7</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>The Frogs</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knfyg7</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1knfpor</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Anything to stop me biting my nails. I've never had my nails done before so this was a new thing I tried today. Done by Sarah at the_nailcircus afflecks Manchester</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knfpor</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1knfegr</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Holo Taco - Vitamin Glow!</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knfegr</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1knd811</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>contact dermatitis</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1knd811/contact_dermatitis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1knexwk</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>I really love the designs with draws and glitter but I feel they don't look good on me because I have so many tattoos, I always choose one color or baby boomer. I know I am boring.</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knexwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1knei4w</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Need nail ideas for an 80's themed party.</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1knei4w/need_nail_ideas_for_an_80s_themed_party/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1kne3fq</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Just wanted to share my new desk setup and work space</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kne3fq</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1kne0y0</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Obsessed with this😍</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8zfh5b9dz0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1kndce6</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Advice on beginner products for gel pedi/manicure welcomed!</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0mzfcug8z0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1kncgxz</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>A years improvement</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kncgxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1knc2xe</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>first attempt using nail brush</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knc2xe</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1knc0kk</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>I.D. Help With Cat Eye Gel Polish Bottle</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1knc0kk/id_help_with_cat_eye_gel_polish_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1kn8fpg</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Home gel set- advice on pinky?</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn8fpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1kn8qq7</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>An hour after this photo the bow got ripped off</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrlmjgouay0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1kn2fnj</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Can anyone suggest some pre-decorated hard gel nail brands?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kn2fnj/can_anyone_suggest_some_predecorated_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1knarky</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Why does my polish separate at the base?</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knarky</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1kn6m06</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Rings of Fire?</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn6m06</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1knatb0</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Tried a new salon while traveling … is the cuticle work isn’t as bad as I think ??😭</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/enzkro97qy0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1kn7x79</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Gel x tips</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kn7x79/gel_x_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1kna6z3</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>first time getting my nails done...</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kna6z3/first_time_getting_my_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1knavu0</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Gel Polish Peeling! Help!</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vd25ogjoqy0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1knatjc</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Life after Acrylics</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1knatjc/life_after_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1knahmi</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Nails my friend did for me</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwl6i7utny0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1knah08</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>New set done today….. getting de autumn vibes….</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2apqtogpny0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1knadja</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>How to do gel x at home?</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1knadja/how_to_do_gel_x_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1kna7ea</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Nude nails</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kna7ea</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1kna6np</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Are these too thick or fine?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/586y71xnly0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1kn9v7y</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Pedicure</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn9v7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1kn9p50</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Gel nails</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kn9p50/gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1kn9o8w</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Ideas for nail tech gifts?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kn9o8w/ideas_for_nail_tech_gifts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1kn9isx</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Is this color more of a blue or purple?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn9isx</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1kn9g98</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>*Obnoxiously* pink and I'm here for it 🩷</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ag5nvjk7gy0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1kn94rb</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>New colour, new me ☺️</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03fj2g1udy0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1kn83ou</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Bio gel ruined my nails.</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn83ou</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1kn7rub</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Graduation Nails!</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn7rub</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1kn6xdw</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Obsessed w/ this blue cat eye</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38i1kd8uvx0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1kn69ar</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Obsessed with these fr</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3kmbfmrpx0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1kn5ylf</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>First set in a while. Decided to go classic with a little razzle dazzle for spring. 🌷🪻🌻</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwh6zidsmx0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1kn5rn8</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Colourful nails ~</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncouor7tkx0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1kn58bn</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>I know it’s mostly girls</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kn58bn/i_know_its_mostly_girls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1kn4whu</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Tried to do black/red Ombré, how did I do? Any pointers?</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kc1c1q7bx0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1kn4k51</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>First time gelx!</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn4k51</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1kn4dn0</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>New gel set! I had to go shorter because I got a job (yaaay 🎉) and I need to type a lot.</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn4dn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1knunaj</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Non gel magnetic polish</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1knunaj/non_gel_magnetic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1knsisi</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Fake Dating: my first BKL</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/azx6vmx7q21f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1kns55n</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>my perfect nude polish??</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kns55n</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1kns3qw</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Lurid Faves</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kns3qw</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1knry0q</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>I’m SO GLAD I bought this polish!</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07ti1b46k21f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1knrooz</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Is anyone able to share swatches of both BKL’s Choose Life and Clionadh’s Psilocybin/Beocystin/Psilocin?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1knrooz/is_anyone_able_to_share_swatches_of_both_bkls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1knrhqp</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Root of All Evil is my favorite nail polish of all time 🪲</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knrhqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1knr61b</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>I changed my nail shape!</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knr61b</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1knqw8g</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Wowza</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jq6bhsjw921f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1knqq8j</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Lost in Love's Labyrinth ✨</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knqq8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1knqmc0</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>How do you do your nails in an insanely humid climate?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knqmc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1knq7cf</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Pina colada me</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knq7cf</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1kno4t1</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Koi Fish!</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gk09knauj11f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1kno01t</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>I miss Illimite every day</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kno01t</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1knnxlj</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Neon Polish Recommendations?</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1knnxlj/neon_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1knnkqw</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Fawning over Bluebird’s Lacquer’s Scope It Out</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knnkqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1knn9zs</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>ombré - what am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymm8rk5vb11f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1knn6nv</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Puglia Perfect ✨✨✨</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irsle4l2b11f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1knmzvy</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Not sure what’s harder- painting a moving target or trying to convince them to take a picture.</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knmzvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1knmaqu</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>If you had $100 what would you buy?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1knmaqu/if_you_had_100_what_would_you_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1knm5in</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Black and gold</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqmpo5t2211f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1knlilf</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Nail grows out weirdly</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knlilf</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1knl6tm</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Cleaning up excess nail polish after drying</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1knl6tm/cleaning_up_excess_nail_polish_after_drying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1knk5gj</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Please help me find a polish with similar colors to this wasp</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r286fu7ul01f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1knjntk</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Finally getting to my preferred length!</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knjntk</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1knj3cm</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Beginner magnetics - Aurora Borealis by Paint it Pretty</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d3qbrwf3e01f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1knigrm</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>new set i hand painted yayyy</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knigrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1knhtq8</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Tips for aura nails?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9j8447t401f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1knhq5c</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Threw some of my unused polishes together and ended up with a stunner!</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i6qi05nt301f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1kngejv</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Best brand for chrome/metallic polish?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kngejv/best_brand_for_chromemetallic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1knf83a</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Keyboard Recommendations</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1knf83a/keyboard_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1knet99</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Crappy cuticles, painted fingers idc I'm obsessed!</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ga8fwluiz0f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1knemdk</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Showin' off my shiny white French tips. I absolutely love 'em so much! 🥰😁✨️💕🤍</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rc3obaihz0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1knehi1</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>My biggest haul yet 🥲</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knehi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1knd6bi</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Im beautiful, im mad ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knd6bi</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1knd0wu</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>[Cirque Colors] Groove Thing</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knd0wu</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1kncwph</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Ethereal Lament 💙🦋</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kncwph</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1knc66h</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Finally found the perfect lighting for this polish</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jfpguc900z0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1knbz7f</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Having a bad week of manicures</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lymomw6kyy0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1knbtox</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Did I develop a gel allergy? Or is it maybe just the new product I got?</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knbtox</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1knbrne</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Pank.</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knbrne</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1knbo2a</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Bar magnet + horseshoe semi-fail</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knbo2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1knbnrn</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Finally got around to trying my most anticipated polish in my collection 🪩</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y9ef6ni9wy0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1knbl17</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>doing crone shit 💓</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knbl17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1knbh5y</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>cabochon palette!</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/25qszbtyuy0f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1knakkq</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Latest pink mani vs my first one 😅😅</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knakkq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1knaii8</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Mooncat + Sassy Sauce out on the TN trails!</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knaii8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1kn9vhj</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Spring Emotions 🌱</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4plpdkpejy0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1kn9s5m</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Indestructible nail top coats</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kn9s5m/indestructible_nail_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1kn9bpt</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>🌿 herbalism 🌿</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn9bpt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1kn8l4h</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Sally Hansen</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn8l4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1kn8fdm</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>This is a longshot, but please help me find an essie/OPI colour</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn8fdm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1kn7ktu</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>if i buy before the price increase it’s basically on sale right???</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rklyzsi1y0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1kn70dc</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>My attempt at stained glass</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn70dc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1kn6lqz</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>The HoH But Make It Red Challenge</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn6lqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1kn0a5f</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>DUPE???</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kn0a5f/dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1kn5qfh</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Does this colour suit me?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn5qfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1kn5aue</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>A few questions for beginner doing my nails.</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kn5aue/a_few_questions_for_beginner_doing_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1kn59an</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Autumn zing</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn59an</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1kn518y</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Pastel one coater</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ld11lxmqcx0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1kn3rtw</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Looking for polish similar to this one</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kn3rtw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1knswpj</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Winnie The Pooh! 🎈🐝</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knswpj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1knspe5</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Really happy with how clean my characters are coming out! Here is Goro Sajuro ☺️</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fnoeja96s21f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1knsj8o</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Recently did these magnetic hearts nail art</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/843t0oy4q21f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1knrsli</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Next batch</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knrsli</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1knrn0i</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Cloudy top coat</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1knrn0i/cloudy_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1knr3mw</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>custom press on set :)</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2n9xu0cxb21f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1knqg6a</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>How do I seal these? Top coat needed?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knqg6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1knpsu4</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Patchwork Quilt</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knpsu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1knntms</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Pink🩷💖</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swrddhvwg11f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1knnsar</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Homemade sunflower art :)</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knnsar</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1knnhgk</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Blue🌠💙</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7oxxxttrd11f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1knmsbp</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Did a blue set after a longtime. Let me know if you guys wanna see how it looks on hands</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knmsbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1knl839</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>New custom set</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q90trjdcu01f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1knkfyb</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Where's the honey? Should I stop?</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2744fq1o01f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1knkfef</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>PROGRESS!!</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkhst2cyn01f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1kngdie</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Thank you all for last weeks feedback!</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kngdie</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1knfviy</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Attempt at fire nail art</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knfviy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1knfuzv</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Butterflies reverse stamping nail art</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/MHQyBbsaaEs?si=b4ds4TmiVGRwBa85</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1knfraf</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>First ever time having my nails done.</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4992g3uopz0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1knegt5</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>💜💜💜</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05u1dblegz0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1kne111</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Pink and butterflies</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kne111</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1knahwh</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Luxa Gel on natural nails by @kalsrebelliousnails on IG</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knahwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1kn5vdg</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Mixing new colors with Neonail UV polish</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kn5vdg/mixing_new_colors_with_neonail_uv_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1kn3koc</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Chrome isolation WONT ISOLATE???</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kn3koc/chrome_isolation_wont_isolate/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat May 17 08:10:39 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_18.xlsx
+++ b/data/collected_data/2025_05_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1042"/>
+  <dimension ref="A1:C1233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18147,6 +18147,3253 @@
         </is>
       </c>
     </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1konfyg</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Nails of 2025 so far, courtesy of my nail artist</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1konfyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1komxuq</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Transparent tips 🧊</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1komxuq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1komwuf</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>My wedding is a little over 12hrs away. Viking/goth wedding. It took a little over a hour for me to finish my nails..</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n537znkmja1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1komrq1</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>First try doing nails!!</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1komrq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1kolvkg</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Advice on press on sizing please!</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kolvkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1koloul</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>What nail shapes could look good on me?</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1koloul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1kokqav</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>My second MANicure</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kokqav</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1kokpks</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Galactic 💅</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q0dzrgr3u91f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1kok779</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Which One is Your fav?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2iyh26slo91f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1kokolb</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Simple French .</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlnbgo1tt91f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1kokm4l</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Should I go back and have them corrected?</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kokm4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1kok5ju</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Guess how long these took me 🥲</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kok5ju</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1kojy61</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Tried doing a stained glass design🌹✨</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i0a2dqw5m91f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1koithq</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Don’t want to get my nails done again</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1koithq/dont_want_to_get_my_nails_done_again/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1koj5fi</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>new nails 💋</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usaqkyt4e91f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1koiopw</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Can finally post here after so long of lurking and 5 years nail free 🩷</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5f3nmpdf991f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1koio87</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Niece fixed nails</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1koio87</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1koilpj</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Got frenchies today 😍</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0wewlwl891f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1koikeb</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>what do you think?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jy47t599891f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1koctdk</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Remedies for press-on nail pain?</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1koctdk/remedies_for_presson_nail_pain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1koi41s</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>EDC inspired ✨</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1koi41s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1kohux0</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>First time doing press ons in 4 months</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kohux0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1kohjlc</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>To dremel or not to dremel.. that is the question!</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22iqvebay81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1kofali</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Toe nail problem</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kofali/toe_nail_problem/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1kohjkn</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Ombre Leopard Print💖🐆</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ziurxo7ay81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1kohgoj</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>My third set of press-ons!!</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kohgoj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1kobeyr</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>handpainted nails inspired by local flora!!</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kobeyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1koazzl</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Over cut the skin beside my nails</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1koazzl/over_cut_the_skin_beside_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1koav31</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>using gel-x for press ons - tips welcomed</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1koav31/using_gelx_for_press_ons_tips_welcomed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1kogbn7</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Tried a brand I know my skin doesn’t like regretting it now.</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/096jo4mqm81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1kob7s9</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Nail drill catching on nails</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kob7s9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1ko8jk5</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Soft builder gel fill?</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ko8jk5/soft_builder_gel_fill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1kobf9d</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Usual place was closed, walked into a random salon an hour before close</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qr8uuj1yh71f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1kobha5</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Can someone help me decided on a nail shape for my appointment</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5ds1jhdi71f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1kodqmm</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Advice Needed</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kodqmm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1kof4hq</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Can Soft Gel Full Coverage Fake Nails be used with nail glue or adhesive tabs?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kof4hq/can_soft_gel_full_coverage_fake_nails_be_used/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1kof4rh</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Gel nail fell off 💔</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egh37l2xb81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1koglv6</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>My inner crow is DELIGHTED</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pyczx6mep81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1kogogo</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Emergency Press-Ons</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/327pjws2q81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1kogcvx</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Decided to do something simple</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kogcvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1kog3np</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>my all time favorite DIY mani 🌼</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kog3np</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1koforv</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Russian style manicure</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1koforv/russian_style_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1kofl36</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Festivals nails 🤘</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kofl36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1kofjak</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Watermelon 🍉</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kofjak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1kofixv</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Second at home mani</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmhbnduef81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1kofbaa</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>First time doing mine in forever!</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kofbaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1kofa6e</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>first time getting nail art!</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etcnm83ad81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1koemvc</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Please help!!! I got short acrylic stilettos, but on my clubbed thumb, it just looks like a big weird triangle.</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxrne7om781f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1kof3c3</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Is there any way to sharpen a cuticle fork?</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6atrmlrkb81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1koevtf</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Fire</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/alw4rg0t981f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1koe5ei</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Press on help?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1koe5ei/press_on_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1kodm9l</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Graduation nails!!! Matching pink pedi not pictured</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zwwxy86z71f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1kodbrj</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>3.5 wk appointment on Wednesday. Anything I can do to protect the natural length until then?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dncsnesrw71f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1kod1e9</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Started going to an independent nail tech 🖤</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kod1e9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1kocudi</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aej694xvs71f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1kocrq5</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>recent biab set!!</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qd2rpwas71f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1kocjin</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kocjin</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1koc5pe</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>what’s wrong with my nails?</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1koc5pe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1kobf8h</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Builder gel</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kobf8h/builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1koaql0</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>The perfect Blurple</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1koaql0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1koapzr</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>i’m so obsessed!</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y677bgwkc71f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1ko9xmm</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>My new set! 🥰🥰 All pearly and girly! 🩷</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5m753jbo671f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1ko9smj</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Soft, feminine, and impossible to ignore, want more? 🤍✨️💅</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xonuq0km571f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1ko9qhs</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>I do them myself (gel) how do they look</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvrq8uf2571f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1ko98gv</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Cheetah print has been super popular lately!</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko98gv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1ko96ac</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Convincing Press-Ons?</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko96ac</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1ko95cv</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>I am obsessed with my new nails</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fk62q69n071f1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1ko8itz</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>My 3rd set!!!</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmj59gmwv61f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1ko8fef</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>🦩 Cirque Colors Flaminglow 🌞</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko8fef</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1ko8e2b</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Please rate my nails</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko8e2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1ko7ohm</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>I love my nail artist!!!!</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko7ohm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1ko7lim</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>I live for a good gold moment</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko7lim</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1ko7jiq</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Not spring nails...but still super cute 🥰 press ons are my favs</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko7jiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1ko7a47</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Cat eye</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z52uzl6zm61f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1ko1ezi</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Cracked thumb</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko1ezi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1ko0v1i</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Should I wait to get them done again?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kyevazmb51f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1ko0a66</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>BFF’s Wedding in 2 Weeks, What Nails Should I Get with my Hand/Finger Type</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1da0cyqt651f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1ko3noo</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>INSPO PIC - NEED HELP! Credit to @studiogesaa on TIKTOK</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mv5ehw4nw51f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1ko3yp8</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Best builder gel to use on myself?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ko3yp8/best_builder_gel_to_use_on_myself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1ko6jka</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Applying acrylic tips</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ko6jka/applying_acrylic_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1ko5kj5</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>In love with my vacay set🌿✨</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dodurxtka61f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1ko4ntd</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>First time doing long ones myself ❤️</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko4ntd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1ko4jq2</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Love light purple nails in the spring. This one is “don’t toot my flute” so cute!</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rnmdhr2361f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1ko49s6</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Tried something a little more difficult!</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gthgfjo2161f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1ko3u3n</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Cowboy nails made by me 🤠</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38b64ztxx51f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1ko3h3v</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>I loved this result</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xt3dtmav51f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1ko26cu</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>New nails 💅</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icf5h8lql51f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1ko1vq5</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>A dangerous girl</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycnl8s0jj51f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ko1ved</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Holiday stilettos (gel-x)</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko1ved</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ko1n8x</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Sage set 🍃</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hiymzvrph51f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1ko1gpa</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Tropical fishing lure ls unlocked.</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko1gpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1ko114f</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>bday nails check ♥️ 🖤</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko114f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1ko0oll</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>My new set</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0to57ap6a51f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1ko0mxm</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Fresh spring set 💜</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhhskozs951f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1ko04h5</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>I love a deep red</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcbx36ti551f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1ko04c7</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>sky malachy dragon themed nails 🩵</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko04c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1ko03ds</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Some favourites from my collection! Happy to show swatches of any if anyone is curious.</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko03ds</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1ko01pf</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko01pf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1knzzcd</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Just wanted to share</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knzzcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1knzfrs</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>i need advice on taking care of my nails. im so new to this. they're not pretty at all</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knzfrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1kon9v5</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>ILNP Rosalie</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kon9v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1kon7ns</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>The Neutral Nude</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kon7ns</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1kokzp1</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Disappointed by mooncat but maybe it’s the top coat?</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kokzp1/disappointed_by_mooncat_but_maybe_its_the_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1kokw40</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Y'all I messed up</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kokw40/yall_i_messed_up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1kokdlo</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>went cherry picking the other day 🍒</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kokdlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1kok845</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Orange is not my colour, I said</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kok845</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1kojsww</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>our colors are SCARLET AND CREAM (minus the cream)</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nqjjcgpmk91f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1kojlwh</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Tried to do lacquer glass nails</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h8ya6kfoi91f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1koj6lu</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Help me finalize my first ILNP order please? 🥺 Dupes for Mooncat Stolen Kiss?</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1koj6lu/help_me_finalize_my_first_ilnp_order_please_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1koj6ay</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>an (early) midsummer’s dream</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6eay1ijde91f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1koj5cv</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>ISO cyan/bright red shifty polish?</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1koj5cv/iso_cyanbright_red_shifty_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1koimm8</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Best NON QDTC?</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1koimm8/best_non_qdtc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1kohs7n</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Mermaid Bait</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kohs7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1kohku8</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>What brands/makers do a particular type of polish best?</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kohku8/what_brandsmakers_do_a_particular_type_of_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1kohgc4</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Top coats for a smooth glossy finish over glitter/flakie polishes?</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/np2rwuxex81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1kohczi</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Has anyone successfully duped Kathleen and Co Rosary Pea or By Dany Vianna/Vanessa Molina/Whatcha Labradorite?</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kohczi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1koha69</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Deep Space is everything</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/elczfm9qv81f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1kogu0v</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>🌹Rose Jam by Potion Polish❤️</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whwt8pwhr81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1kogoem</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>My thumbs tend to develop horizontal cracks below the free edge, is using nail repair glue likely to cause an acrylate allergy like gel can?</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kogoem/my_thumbs_tend_to_develop_horizontal_cracks_below/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1kofbzr</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>My bookish manicure today</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kofbzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1kofapj</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>The Last of Them Collection available now! www.apocalypsepolish.com</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4zom9u8d81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1kof9ve</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>🍓 strawberry nails🍓</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kof9ve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1koetts</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Rainbow of Cirque Colors Jellies</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5icx6mb981f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1koemz8</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Found this in the nba sub. As a hardcore basketball nut, this makes me happy.  There’s a couple of players who paint their nails in the league, love seeing more men embrace polish.</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://streamable.com/zwu0cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1koek04</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Any Chance Blades of Frontiers and FFS will come back?</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1koek04/any_chance_blades_of_frontiers_and_ffs_will_come/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1koecqr</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>What's up with Out The Door top coat? I can't find it at Sally.</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1koecqr/whats_up_with_out_the_door_top_coat_i_cant_find/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1koeazp</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Jared McCain announces that he is launching his own line of nail polish</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://streamable.com/zwu0cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1koe2dr</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers 10th Anniversary Collection Drop!</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uckgkvpk281f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1kodl3c</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Mooncat - Access Denied</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kodl3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1kod6ff</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Polish finishes</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kod6ff/polish_finishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1kobssn</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>File too much for a Russian manicure?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kobssn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1kobcw8</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Barbra from ILNP is the most transparent owner out there who genuinely cares about her customers and for that reason she deserves all the love and support</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/idqjer3hh71f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1kob35z</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Seriously this topcoat is the glossiest!</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kob35z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1kob056</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>First attempt at marble nails!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kob056</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1koapw0</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Favorite top coat?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q16abuikc71f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1koahmx</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Cirque Groove Thing with Marsala Jelly accent nails and layered ILNP fairy dust</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3522qfua71f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1koaght</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Smitten with “Smitten.”</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1koaght</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1ko9o7y</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Jelly sandwich obsession</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko9o7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1ko8w4q</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Butterfly wings 🦋</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko8w4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1ko8v4g</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Raise Octaves</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko8v4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1ko8uya</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Brick and mortar stores for indies/ boutiques? Also Atomic/ Minneapolis question</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ko8uya/brick_and_mortar_stores_for_indies_boutiques_also/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1ko8d7g</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Do you see the pink?</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bfw6j03pu61f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1ko8bjv</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>🦩 Cirque Colors Flaminglow 🌞</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko8bjv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1ko6ldx</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>My hands are healing from compulsive picking and nail pulling up thanks to you all!</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko6ldx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1ko6o28</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>please help me find this shade!</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko6o28</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1ko7kxh</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>If they only knew the you that we know 🤯</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko7kxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1ko71a0</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Miz Claws 💙🦋</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvaz46h5l61f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1ko70cr</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>How do you organize your polishes?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ko70cr/how_do_you_organize_your_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1ko6ura</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Barbie Vibes</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko6ura</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1ko6pap</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Serpents of Eden vs Reminisce?</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ko6pap/serpents_of_eden_vs_reminisce/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1ko5r5o</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>gradient skittle looking 🌅</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko5r5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1ko5l0g</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>The many faces of Pigment Of My Imagination</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko5l0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1ko5jut</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Solid neon blue?</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6kt9qjfa61f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1ko580n</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Q: for Square/Coffin shape nails</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n90edt20861f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1ko477i</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>AMERIICAN REQUIEM Mani</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l8hjwqjj061f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1ko3ed6</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Squish</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqnfz8oqu51f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1ko2xyp</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Eurovision nails with flags for every country of my top 10 past winners 🇨🇭🇸🇪🇮🇹🇬🇷🇫🇮🇩🇰🇱🇺🇩🇪🇬🇧🇳🇴</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko2xyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1ko2p4v</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Why do my nails keep breaking?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko2p4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1ko21an</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Molten Lavender - A Comparison 🔥🪻</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko21an</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1ko1vc0</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Bikini on a Misty Mountain Top</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko1vc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1ko1qkt</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Obsessed with psilocybin...And Fire</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b4m4v59fi51f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1ko1pp7</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Spring nails!</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko1pp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1ko1n3d</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Could I send you a photo of my bare nails after 4 months of gel acrylics to get your opinion?</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ko1n3d/could_i_send_you_a_photo_of_my_bare_nails_after_4/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1knzolt</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>New brand: Funny Business Lacquers</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1knzolt/new_brand_funny_business_lacquers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1knz666</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Whom will I see at Atomic Polish's polish-making drop-in at Art-a-Whirl in Minneapolis this weekend?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/atomicpolishmn/p/DJmh6sxtA2n/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1knyth8</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Chipping polish, redo manicure or another topcoat?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1knyth8/chipping_polish_redo_manicure_or_another_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1knx76u</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Recently did these magnetic hearts nail art</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wnticgy3c41f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1knwr7f</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>I really love this color! 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1knwr7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1knek3f</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Can I make matte look glossy?</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mh2rg9y1hz0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1konvkk</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>pls help me how to chrome isolation and what am i doing wrong</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjd2hcvjva1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1komx36</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>My wedding is a little over 12hrs away. Viking/goth wedding. It took a little over a hour for me to finish my nails..</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q2x9wjjpja1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1kokz9a</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>nails i did this week</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqjv6iy3x91f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1kokeam</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>EDC nails my wife did this week!</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ruiy400qq91f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1kojqth</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>New to the art</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kojqth</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1kognoc</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>I LOVE THESE SO MUCHHHH</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qzgelbvp81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1kofz7g</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>You can say...we ate</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kofz7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1kofrwr</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Tutorial request</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3x56yynh81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1kofi1b</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>HELP what design should I do</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2urz1i27f81f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1kocy1b</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>I want to go to the beach with these beauties🏝️👙🐚</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qq6kvnqpt71f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1kobmpu</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Independent nail artists in eldorado KS?</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kobmpu/independent_nail_artists_in_eldorado_ks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1kob41r</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>My first attempt at marble nails!</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kob41r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1ko78lm</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>MIX ♥️ 💜</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zk8smaom61f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1ko4z3z</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>First time doing someone elses nails</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4hy644i6661f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1ko3kub</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Beautiful design made with gel</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6l4e3r22w51f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1ko2igb</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>I’m not sure what to call this style but I love it!</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2le9zn9o51f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1ko2ibm</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>I might have to do the pinky in a whole set.</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko2ibm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1ko1zq6</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>character nails!</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko1zq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1ko1wxg</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Husband hates this set but I love them!</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko1wxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1ko1f8k</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Arcane nails made for a friend what yall think</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ko1f8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1kny4wt</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Why did my design „melt“?</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qblxgaom41f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1knguif</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>NailsArt 😍😍😍</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwbqz0zkxz0f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun May 18 08:10:49 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_18.xlsx
+++ b/data/collected_data/2025_05_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1233"/>
+  <dimension ref="A1:C1407"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21394,6 +21394,2964 @@
         </is>
       </c>
     </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1kpdqlh</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>How much would you pay?</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1agmaiudlh1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1kpdmgx</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>New DIY nail options?</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kpdmgx/new_diy_nail_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1kpdhbj</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Been loving doing my own nails at home recently. Here’s some sets I’ve done! Far from perfect but they’re so much better than when I started</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kpdhbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1kpcik8</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Guy trying med/long almond shaped acrylics</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thts3wjr6h1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1kpcf2a</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Flame polygon</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1gfwrmn5h1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1kpb2dj</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>first attempt at diy gel nails</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kpb2dj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1kpayn0</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>This nail oil container is so easy to refill and has a brush!</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kpayn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1kpayfr</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Homemade press ons,</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ohr8u6nipg1f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1kpayas</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>My “Immaculate” bird catcher nails</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kpayas</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1kpay35</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Wifey just did this set today</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kpay35</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1kp90ix</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>First attempt with French tips</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xg0ucfin5g1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1kpabwa</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Shopping on Etsy</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kpabwa/shopping_on_etsy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1kpatoq</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>First time doing my own gel nails with no efile. Pretty happy with the way they came out.</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjg6xlh5og1f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1kpar86</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Fun design I enjoyed doing!</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kpar86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1kpamxy</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>First time trying cat eye 😼</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z20we4y5mg1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1kpaj5s</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Press on nails grew my nails longer and faster than acrylic nails. This is after 3 weeks</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmz7c3w3lg1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1kpaiu0</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>First time with builder gel. Obsessed with my nail lady’s work!</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxj0soj0lg1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1kpa036</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>I finally figured out isolated chrome 🥹</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28iv3v2nfg1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1kp9ttn</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Went with a PNW coastal theme for this set</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b17jdj9sdg1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1kp9hur</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>rosy moments🌸✨️🩷</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp9hur</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1kp96ti</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>thought these were fun lol</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp96ti</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1kp91n8</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Minecraft Nails to Match my kids Birthday Party</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wb3eelay5g1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1kp8dng</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Dots and 3D nails</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp8dng</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1kp7s7o</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Are my nails okay??</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp7s7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1kp7nsw</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Work beats the fuck out of my nails, but at least the lighting is nice!</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp7nsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1kp7l1h</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Summer nails!💚</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp7l1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1kp7k13</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Red will always be the most delicate color for my nails.</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tuiwgq7drf1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1kp7gty</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>New Set, Who Dis?</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ummdkk4iqf1f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1kp7efa</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Why do I always get these white spots on the same parts of my nails?</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i76hdt2upf1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1kp72yi</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>how to remove dip powder nail extensions?</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kp72yi/how_to_remove_dip_powder_nail_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1kp6ur3</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Gel extensions keep snapping??</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp6ur3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1kp6mei</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>It’s a rare treat when I get nails, but these were some of my favorite</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4uz2ww8if1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1kp1lo7</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Having the most fun reproducing album covers on my nails! This time it's Tycho and Jon Hopkins!</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp1lo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1kp2knv</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>What i asked for vs what i got.</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp2knv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1kp3ebf</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>What to do with a metric shit-ton of extra nail tips?</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/in1k9aqoqe1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1kp50pm</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Really wanna start doing my nails but I have some DUMB questions</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kp50pm/really_wanna_start_doing_my_nails_but_i_have_some/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1kp6fy4</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Just started doing my own poly gel nails at home.</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp6fy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1kp6fl5</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>I realized today my thermal gel polish matches the Hibiscus in my garden 🌺 ❤️</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txy4fdnxgf1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1kp65hn</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>First time getting my nails done!</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp65hn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1kp50kp</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>🩵🖤🩶 (done by @nailsbyghostie)</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp50kp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1kp3kha</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Builder gel question</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kp3kha/builder_gel_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1kp4n2q</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Chrome never disappoints 💗</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp4n2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1kp4hql</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Remove color from gel x extensions</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kp4hql/remove_color_from_gel_x_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1kp43qp</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp43qp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1kp3yxn</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Mother’s Day nails</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytb28oodve1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1kp3vwz</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Just a Dad trying to learn to paint his daughter's nails.</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kp3vwz/just_a_dad_trying_to_learn_to_paint_his_daughters/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1kp3sbq</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>More natural nails</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp3sbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1kp3o6n</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Gopher pose anyone? 😛</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9sz7pmtxse1f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1kp3et5</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Cherry red for summer!</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp3et5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1kp377d</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Help, there’s a certain pink I want but I can’t find the right shade</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6aymi946pe1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1kp3633</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>My natural nails</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp3633</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1kp32qg</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>new set i got done today☺️</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvs0vou6oe1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1kp2yyl</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Cute and simple 🌸</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5aurdadbne1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1kp2wfm</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>First time doing my own dipping manicure!</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp2wfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1kp2s5c</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Acetone Substitutes?</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kp2s5c/acetone_substitutes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1kp2kd8</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Are my hands too masculine, nail beds too wide?</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp2kd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1kp2cu4</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>New mani what does everyone think?</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhdsagubie1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1kp23yd</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Woodpecker nails</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/memv8idcge1f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1kp1m5m</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>First Ever Manicure (biab)</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp1m5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1kp1kg8</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Glitter Stiletto Nails</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6x79xr1ce1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1kp1c85</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Natural Nail Growth Journey!</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp1c85</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1kp1hwn</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Can you tell which is my non-dominant hand?</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp1hwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1kp1g2j</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Juicy</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmq7vby2be1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1kp149u</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>My summer themed DIY nails with regular polish!</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp149u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1kp0yas</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>What shape is best</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp0yas</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1kp0y0d</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>I’m in looove with this set</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hs2plw477e1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1kp0st1</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Please rate my nails</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp0st1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1kp0nxs</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>My pink opals!</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/weab4dd15e1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1kp0f37</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>My nail tech was so proud of the snakes</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2g6mm5mz2e1f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1koysk4</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Which is more beginner friendly - BIAB or Gel-X?</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0tw25fbqd1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1kp097p</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Progress Post from Nikki Nailed it - Nail Tech In Training</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp097p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1kp0c2l</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>My second hybrid gel set</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp0c2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1kp09w2</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Barista nails</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kp09w2/barista_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1kozwz5</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>DND “first kiss” w mirror chrome</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kozwz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1kozu09</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Sometimes you just need a classic red nail</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0aiv3afmyd1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1koznde</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Lost my polish and then broke that nail within maybe two hours</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6ejvft6xd1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1kozfkh</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Opinions please</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kozfkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1koze47</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>New ones on me by me 😍</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwfkl9r5vd1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1kozar9</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Can you tell which is my non- dominant hand?</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kozar9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1koz7k0</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Natural looking press ons</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1koz7k0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1koz6ap</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>almond shape 🤍</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7pomfajtd1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1koyzf9</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Advice requested - BIAB or gel-x for complete beginner?</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wcjl16wxrd1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1koyreu</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>First time Gel X</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71qbs7paqd1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1koyrb2</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Growing out nail advice?</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1koyrb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1koyilt</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>My artist amazes me everytime!</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c7jelfpcod1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1koyfn3</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Attempted tortoise nails🐢</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tb4evcwpnd1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1kox58c</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Stitch nails</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4r9ghydjdd1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1koy0u7</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Lamp for DND?</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1koy0u7/lamp_for_dnd/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1koxy0i</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>I did my own acrylic for the first time!</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1koxy0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1koxarw</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Breakage :( do I file all of them down? Suggestions?</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1koxarw/breakage_do_i_file_all_of_them_down_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1koxan9</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Losing any confidence I had with doing nails, do these look ok?</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sm2l4cwred1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1kox9db</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Simple cat eye</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4glif8hed1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1kowma4</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>I did my mom's nails for Disney world</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lm368phg9d1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1kowk9i</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Sistaco wine + candle 2:1</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kowk9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1kouun2</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Advice for Overfiled Nails</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kouun2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1kov58c</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Some progress! First picture is from February, last pic is from this am,  my latest set ❤️ any tips?</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kov58c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1kotm0v</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Nail makeover</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kotm0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1kov6fq</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>How do I get rid of these?</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mmvrw08yc1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1kowa59</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>I promised to post em on so…</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a89dp76u6d1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1kow54y</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Nail shape advice</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kow54y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1kpetp5</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>My 1st summery mani! Its giving princess fiona</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5q1xc55zh1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1kpelwa</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Inspired by Strange the Dreamer</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kpelwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1kpd312</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Fingertips stained from nail Polish??</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kpd312</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1kpbk2v</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>✨️vacation nails✨️ but I live in the tropics so they're just normal nails to me</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kpbk2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1kpb616</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a997b4sprg1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1kpb25h</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>This nail oil container is so easy to refill and has a brush!</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kpayn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1kpapyx</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Good Morning, Garden Path!</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7n4jvfvrmg1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1kpaldq</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Frosted Metals</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kpaldq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1kpaeq7</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Uno Mas Colors Launch - 5/22/25!</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kpaeq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1kp9pw6</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Appreciation post 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kp9pw6/appreciation_post/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1kp93uh</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>ILNP Flower Child over White/Lavender/Light Blue/Beige</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kp93uh/ilnp_flower_child_over_whitelavenderlight/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1kp91is</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>It's TOE-TIME!  What's your go-to pedicure color at this time of year?</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kp91is/its_toetime_whats_your_goto_pedicure_color_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1kp86e6</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Welcoming summer, a few weeks early…</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dfb40haaxf1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1kp84vx</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>There was an attempt, rainbow addition</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4draon7wwf1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1kp7gtv</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>non gel dupe of love is in the bare (cool toned milky pink)</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kp7gtv/non_gel_dupe_of_love_is_in_the_bare_cool_toned/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1kp6z2v</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>A perfect yellow for cool undertones</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qik8knwjf1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1kp6ubl</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Y’all - give me recommendations to match this red orange!</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jj3gxthnkf1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1kp6fsz</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Showin' off my shiny white French tips. I absolutely love 'em so much! 🥰😁✨️💕🤍</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpmn9wtzgf1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1kp668o</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Best red glow topper?</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kp668o/best_red_glow_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1kp5jlv</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>I'm so pleased</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp5jlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1kp5fmm</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>When your mani matches your purrmaid PJs</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp5fmm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1kp4p2m</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Everyone NEEDS a Holo Thermo Top Coat in Life 💖</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp4p2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1kp4jra</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Favorite Strengthening Base Coat</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kp4jra/favorite_strengthening_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1kp4c47</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Help with painting nails</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gl9dwzfye1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1kp3otj</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Sparkly nails for tonight’s Beyoncé concert! 🤠🪩</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t9jwo3e2te1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1kp387l</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Which nail shape suits my hands?</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp387l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1kp3795</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Organizing some of my blues and purples</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wq5zvpgqoe1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1kp2y8q</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>BKL Sky-Fire (Velvet)</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0mnr5506ne1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1kp2vgv</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer Pink on Pink</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lh61wbjme1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1kp2r11</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Do nail inks need to be cured or are they air dry?</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kp2r11/do_nail_inks_need_to_be_cured_or_are_they_air_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1koxpys</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>ESC nail art</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1koxpys</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1kp2hb2</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>So satisfying</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp2hb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1kp1yoy</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Bottom coat recommendations?</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kp1yoy/bottom_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1kp1re2</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Thought I'd try Syzygy Boston.</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp1re2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1kp1g39</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Can anyone recommend a clear, matte solution for my nails that doesn't peel?</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdg7dn33be1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1kp0c4z</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>PSA - mega sale at BSG</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kp0c4z/psa_mega_sale_at_bsg/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1kp0a87</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>I think I just found my new fav polish…</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp0a87</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1kp03xp</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Bless Your Heart🤠💖</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zvx9k9mn0e1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1kozalp</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Raise Octaves</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kozalp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1koz3g5</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>ILNP Flower Child in direct vs. low lighting!</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1koz3g5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1koz0qj</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Chunky glitter AND glow?! Yes, please!</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxeauehdsd1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1koyaus</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Drugstore brand PVB free base coat</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1koyaus/drugstore_brand_pvb_free_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1kowh9u</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>{PR} Savage Cindereli by Sassy Sauce Polish 💜✨</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kowh9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1kovvzh</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>How do you take care of your cuticles?</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kovvzh/how_do_you_take_care_of_your_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1kovp0f</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Shattered Glass is so sparkly and shimmery, I can’t stop staring 🤩</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kovp0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1kouwaq</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Cadillacquer - I Would Die For You</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swssf5q1wc1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1kouqrk</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>My patience for magnetics is non-existent, but velvet nails are so worth it✨️✨️</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jtipzj8tuc1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1kouqtk</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>OPI x Wicked - Yellow Brick Road</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kouqtk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1koukub</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Polish Won’t Dry</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1koukub/polish_wont_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1kouka8</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Search continues for best quick dry topcoat....</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kouka8/search_continues_for_best_quick_dry_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1kouial</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>My fav cheap &amp; non-indie polish, Unicorn Tears by Technic</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kouial</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1kotshm</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Had fun with this spring skittle using a different brand for every polish 💝🧡</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ouoalq2nc1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1kot1gp</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Sinful colors Let's talk faded formula and color question</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kot1gp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1kosr95</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Advice on sizing please!</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kosr95</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1koski9</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Inexpensive top coats?</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1koski9/inexpensive_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1kosj57</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Show me your capped tips!</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84ewl7sccc1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1kos3sv</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>will you avoid buying a polish because you hate the bottle?</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5na7r7bi8c1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1korkuv</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Essie Gel damaged my nails?</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1korkuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1korg4l</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Took my PPU polish to Portugal</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1korg4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1kogp5d</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Clambake Dupe?</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kogp5d/clambake_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1kopn4h</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Thoughts on Clionadhcosmetics nail polish?</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwhqq847ib1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1kop6oj</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>what do you do when a polish has a beautiful color but the formula is terrible?</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kop6oj/what_do_you_do_when_a_polish_has_a_beautiful/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1kooef1</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Essie speed setter discontinued in UK?</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcipjfq82b1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1kpengq</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Inspired by Strange the Dreamer</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kpengq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1kpbq37</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Relieve</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vdepgv4sxg1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1kpbpgt</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>My try at butterfly nails</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kpbpgt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1kp9gme</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Another set by me—gold and glam all the way.</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0omvwa3ag1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1kp9c42</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>6 months evolution (from oldest to newest)</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp9c42</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1kp8rm3</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Wifey did this set today</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp8rm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1kp6qvq</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Brand new ombré brush keeps splitting</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwo65u3sjf1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1kp57ys</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Late night nail sessions</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gux3wjt56f1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1kp3uuh</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Slow drying nail polish?</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kp3uuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1kp0aw7</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Stripes!!!</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tngjdv6a2e1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1kp07ce</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Spring / Summer combo nails ☀️</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6u8vwx3i1e1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>